<commit_message>
updated templates to reflect Version 6 Teens Club Report
</commit_message>
<xml_diff>
--- a/teensclub_report.xlsx
+++ b/teensclub_report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PIH\teenClub DHIS2 Integrator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PIH\Event capture DHIS2 excel Integrator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E12963-6F61-4982-9B98-3D903DF7095A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8E51D9-59FD-4848-B4A2-15B54E3D4B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{58AEABA8-2B34-4459-BB0A-42EC3882B367}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>Facility</t>
+  </si>
+  <si>
+    <t>Teen Club - CD4 Drawn</t>
+  </si>
+  <si>
+    <t>Teen Club - Urine LAM Drawn</t>
   </si>
 </sst>
 </file>
@@ -658,20 +664,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{199AE125-C6FD-41F1-8847-0C45D2D2C72F}">
-  <dimension ref="A1:S15"/>
+  <dimension ref="A1:U15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.08984375" customWidth="1"/>
     <col min="2" max="2" width="10.453125" style="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.7265625" style="15"/>
+    <col min="19" max="19" width="8.7265625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="112.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" ht="112.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>31</v>
       </c>
@@ -718,18 +724,24 @@
         <v>30</v>
       </c>
       <c r="P1" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" s="20" t="s">
+      <c r="S1" s="20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="11">
-        <v>45638</v>
+        <v>45272</v>
       </c>
       <c r="C2" s="2">
         <v>95</v>
@@ -773,18 +785,24 @@
       <c r="P2" s="2">
         <v>0</v>
       </c>
-      <c r="Q2" s="14">
+      <c r="Q2" s="2">
+        <v>0</v>
+      </c>
+      <c r="R2" s="2">
+        <v>0</v>
+      </c>
+      <c r="S2" s="14">
         <f>D2+E2</f>
         <v>70</v>
       </c>
-      <c r="S2" s="8"/>
+      <c r="U2" s="8"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="11">
-        <v>45628</v>
+        <v>45262</v>
       </c>
       <c r="C3" s="2">
         <v>45</v>
@@ -828,18 +846,24 @@
       <c r="P3" s="2">
         <v>0</v>
       </c>
-      <c r="Q3" s="14">
-        <f t="shared" ref="Q3:Q15" si="0">D3+E3</f>
+      <c r="Q3" s="2">
+        <v>0</v>
+      </c>
+      <c r="R3" s="2">
+        <v>0</v>
+      </c>
+      <c r="S3" s="14">
+        <f t="shared" ref="S3:S15" si="0">D3+E3</f>
         <v>40</v>
       </c>
-      <c r="S3" s="8"/>
+      <c r="U3" s="8"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="11">
-        <v>45631</v>
+        <v>45265</v>
       </c>
       <c r="C4" s="2">
         <v>50</v>
@@ -881,20 +905,26 @@
         <v>1</v>
       </c>
       <c r="P4" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>0</v>
+      </c>
+      <c r="R4" s="2">
         <v>5</v>
       </c>
-      <c r="Q4" s="14">
+      <c r="S4" s="14">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="S4" s="8"/>
+      <c r="U4" s="8"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="11">
-        <v>45635</v>
+        <v>45269</v>
       </c>
       <c r="C5" s="2">
         <v>15</v>
@@ -938,18 +968,24 @@
       <c r="P5" s="2">
         <v>0</v>
       </c>
-      <c r="Q5" s="14">
+      <c r="Q5" s="2">
+        <v>0</v>
+      </c>
+      <c r="R5" s="2">
+        <v>0</v>
+      </c>
+      <c r="S5" s="14">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="S5" s="8"/>
+      <c r="U5" s="8"/>
     </row>
-    <row r="6" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="11">
-        <v>45635</v>
+        <v>45269</v>
       </c>
       <c r="C6" s="5">
         <v>90</v>
@@ -990,21 +1026,27 @@
       <c r="O6" s="5">
         <v>2</v>
       </c>
-      <c r="P6" s="6">
+      <c r="P6" s="5">
+        <v>9</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>0</v>
+      </c>
+      <c r="R6" s="6">
         <v>24</v>
       </c>
-      <c r="Q6" s="14">
+      <c r="S6" s="14">
         <f t="shared" si="0"/>
         <v>82</v>
       </c>
-      <c r="S6" s="9"/>
+      <c r="U6" s="9"/>
     </row>
-    <row r="7" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="11">
-        <v>45643</v>
+        <v>45277</v>
       </c>
       <c r="C7" s="5">
         <v>60</v>
@@ -1045,21 +1087,27 @@
       <c r="O7" s="5">
         <v>0</v>
       </c>
-      <c r="P7" s="6">
+      <c r="P7" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>0</v>
+      </c>
+      <c r="R7" s="6">
         <v>12</v>
       </c>
-      <c r="Q7" s="14">
+      <c r="S7" s="14">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="S7" s="9"/>
+      <c r="U7" s="9"/>
     </row>
-    <row r="8" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="11">
-        <v>45643</v>
+        <v>45277</v>
       </c>
       <c r="C8" s="5">
         <v>30</v>
@@ -1100,21 +1148,27 @@
       <c r="O8" s="5">
         <v>0</v>
       </c>
-      <c r="P8" s="7">
+      <c r="P8" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>2</v>
+      </c>
+      <c r="R8" s="7">
         <v>7</v>
       </c>
-      <c r="Q8" s="14">
+      <c r="S8" s="14">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="S8" s="10"/>
+      <c r="U8" s="10"/>
     </row>
-    <row r="9" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="11">
-        <v>45628</v>
+        <v>45262</v>
       </c>
       <c r="C9" s="5">
         <v>80</v>
@@ -1155,21 +1209,27 @@
       <c r="O9" s="5">
         <v>0</v>
       </c>
-      <c r="P9" s="6">
+      <c r="P9" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>0</v>
+      </c>
+      <c r="R9" s="6">
         <v>14</v>
       </c>
-      <c r="Q9" s="14">
+      <c r="S9" s="14">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="S9" s="9"/>
+      <c r="U9" s="9"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="11">
-        <v>45635</v>
+        <v>45269</v>
       </c>
       <c r="C10" s="2">
         <v>15</v>
@@ -1211,20 +1271,26 @@
         <v>0</v>
       </c>
       <c r="P10" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>0</v>
+      </c>
+      <c r="R10" s="2">
         <v>1</v>
       </c>
-      <c r="Q10" s="14">
+      <c r="S10" s="14">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="S10" s="8"/>
+      <c r="U10" s="8"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="11">
-        <v>45629</v>
+        <v>45263</v>
       </c>
       <c r="C11" s="2">
         <v>25</v>
@@ -1266,20 +1332,26 @@
         <v>0</v>
       </c>
       <c r="P11" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>0</v>
+      </c>
+      <c r="R11" s="2">
         <v>1</v>
       </c>
-      <c r="Q11" s="14">
+      <c r="S11" s="14">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="S11" s="8"/>
+      <c r="U11" s="8"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="11">
-        <v>45636</v>
+        <v>45270</v>
       </c>
       <c r="C12" s="2">
         <v>25</v>
@@ -1321,20 +1393,26 @@
         <v>0</v>
       </c>
       <c r="P12" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>0</v>
+      </c>
+      <c r="R12" s="2">
         <v>3</v>
       </c>
-      <c r="Q12" s="14">
+      <c r="S12" s="14">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="S12" s="8"/>
+      <c r="U12" s="8"/>
     </row>
-    <row r="13" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="11">
-        <v>45628</v>
+        <v>45262</v>
       </c>
       <c r="C13" s="5">
         <v>10</v>
@@ -1375,21 +1453,27 @@
       <c r="O13" s="5">
         <v>0</v>
       </c>
-      <c r="P13" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="14">
+      <c r="P13" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="5">
+        <v>0</v>
+      </c>
+      <c r="R13" s="6">
+        <v>0</v>
+      </c>
+      <c r="S13" s="14">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="S13" s="9"/>
+      <c r="U13" s="9"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="11">
-        <v>45636</v>
+        <v>45270</v>
       </c>
       <c r="C14" s="2">
         <v>40</v>
@@ -1431,20 +1515,26 @@
         <v>0</v>
       </c>
       <c r="P14" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>0</v>
+      </c>
+      <c r="R14" s="2">
         <v>5</v>
       </c>
-      <c r="Q14" s="14">
+      <c r="S14" s="14">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="S14" s="8"/>
+      <c r="U14" s="8"/>
     </row>
-    <row r="15" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="11">
-        <v>45635</v>
+        <v>45269</v>
       </c>
       <c r="C15" s="5">
         <v>30</v>
@@ -1485,14 +1575,20 @@
       <c r="O15" s="5">
         <v>0</v>
       </c>
-      <c r="P15" s="6">
+      <c r="P15" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="5">
+        <v>0</v>
+      </c>
+      <c r="R15" s="6">
         <v>2</v>
       </c>
-      <c r="Q15" s="14">
+      <c r="S15" s="14">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="S15" s="9"/>
+      <c r="U15" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modified The script to update already captured events so that there are no duplicates created for the same report
</commit_message>
<xml_diff>
--- a/teensclub_report.xlsx
+++ b/teensclub_report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PIH\Event capture DHIS2 excel Integrator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8E51D9-59FD-4848-B4A2-15B54E3D4B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2631DDA-592E-446C-9D66-6EF268330502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{58AEABA8-2B34-4459-BB0A-42EC3882B367}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
@@ -53,27 +53,78 @@
     <t>Ligowe HC</t>
   </si>
   <si>
+    <t>chifunga</t>
+  </si>
+  <si>
+    <t>Dambe HC</t>
+  </si>
+  <si>
+    <t>Teen Club - Actual attendance</t>
+  </si>
+  <si>
+    <t>Teen Club - EAC</t>
+  </si>
+  <si>
+    <t>Teen Club - Males</t>
+  </si>
+  <si>
+    <t>Teen Club - Expected attendance</t>
+  </si>
+  <si>
+    <t>Teen Club-Females</t>
+  </si>
+  <si>
+    <t>Teen Club - Total screened for nutrition</t>
+  </si>
+  <si>
+    <t>Teen Club - Total referred after nutrition screening</t>
+  </si>
+  <si>
+    <t>Teen Club - Total screened for TB</t>
+  </si>
+  <si>
+    <t>Teen Club - TB presumptive cases</t>
+  </si>
+  <si>
+    <t>Teen Club - Total presumptive with sputum collected</t>
+  </si>
+  <si>
+    <t>Teen Club - Total due for viral load</t>
+  </si>
+  <si>
+    <t>Teen Club - Total drawn viral load</t>
+  </si>
+  <si>
+    <t>Teen Club - Total referred for STI</t>
+  </si>
+  <si>
+    <t>Facility</t>
+  </si>
+  <si>
+    <t>Teen Club - CD4 Drawn</t>
+  </si>
+  <si>
+    <t>Teen Club - Urine LAM Drawn</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Zalewa</t>
+  </si>
+  <si>
+    <t>lisungwi</t>
+  </si>
+  <si>
+    <t>Midzemba</t>
+  </si>
+  <si>
+    <t>Matope</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>chifunga</t>
-  </si>
-  <si>
-    <t>Dambe HC</t>
-  </si>
-  <si>
-    <t>Zalewa</t>
-  </si>
-  <si>
-    <t>lisungwi</t>
-  </si>
-  <si>
-    <t>Midzemba</t>
-  </si>
-  <si>
-    <t>Matope</t>
-  </si>
-  <si>
     <t>Neno Parish</t>
   </si>
   <si>
@@ -92,52 +143,7 @@
     <t>Nkula</t>
   </si>
   <si>
-    <t>Teen Club - Actual attendance</t>
-  </si>
-  <si>
-    <t>Teen Club - EAC</t>
-  </si>
-  <si>
-    <t>Teen Club - Males</t>
-  </si>
-  <si>
-    <t>Teen Club - Expected attendance</t>
-  </si>
-  <si>
-    <t>Teen Club-Females</t>
-  </si>
-  <si>
-    <t>Teen Club - Total screened for nutrition</t>
-  </si>
-  <si>
-    <t>Teen Club - Total referred after nutrition screening</t>
-  </si>
-  <si>
-    <t>Teen Club - Total screened for TB</t>
-  </si>
-  <si>
-    <t>Teen Club - TB presumptive cases</t>
-  </si>
-  <si>
-    <t>Teen Club - Total presumptive with sputum collected</t>
-  </si>
-  <si>
-    <t>Teen Club - Total due for viral load</t>
-  </si>
-  <si>
-    <t>Teen Club - Total drawn viral load</t>
-  </si>
-  <si>
-    <t>Teen Club - Total referred for STI</t>
-  </si>
-  <si>
-    <t>Facility</t>
-  </si>
-  <si>
-    <t>Teen Club - CD4 Drawn</t>
-  </si>
-  <si>
-    <t>Teen Club - Urine LAM Drawn</t>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -275,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -329,6 +335,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -666,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{199AE125-C6FD-41F1-8847-0C45D2D2C72F}">
   <dimension ref="A1:U15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -679,61 +691,61 @@
   <sheetData>
     <row r="1" spans="1:21" ht="112.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="18" t="s">
+      <c r="Q1" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="L1" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="M1" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="N1" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="O1" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="P1" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q1" s="19" t="s">
-        <v>33</v>
-      </c>
       <c r="R1" s="19" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="S1" s="20" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
@@ -741,59 +753,59 @@
         <v>2</v>
       </c>
       <c r="B2" s="11">
-        <v>45272</v>
+        <v>45332</v>
       </c>
       <c r="C2" s="2">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D2" s="2">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E2" s="2">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="2">
-        <v>70</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2">
-        <v>70</v>
-      </c>
-      <c r="J2" s="2">
-        <v>0</v>
-      </c>
-      <c r="K2" s="2">
-        <v>0</v>
-      </c>
-      <c r="L2" s="2">
-        <v>1</v>
-      </c>
-      <c r="M2" s="2">
-        <v>1</v>
-      </c>
-      <c r="N2" s="2">
-        <v>65</v>
-      </c>
-      <c r="O2" s="2">
-        <v>0</v>
-      </c>
-      <c r="P2" s="2">
+        <v>35</v>
+      </c>
+      <c r="G2" s="22">
+        <v>72</v>
+      </c>
+      <c r="H2" s="22">
+        <v>0</v>
+      </c>
+      <c r="I2" s="23">
+        <v>72</v>
+      </c>
+      <c r="J2" s="23">
+        <v>1</v>
+      </c>
+      <c r="K2" s="23">
+        <v>1</v>
+      </c>
+      <c r="L2" s="22">
+        <v>4</v>
+      </c>
+      <c r="M2" s="22">
+        <v>4</v>
+      </c>
+      <c r="N2" s="22">
+        <v>0</v>
+      </c>
+      <c r="O2" s="22">
+        <v>0</v>
+      </c>
+      <c r="P2" s="22">
         <v>0</v>
       </c>
       <c r="Q2" s="2">
         <v>0</v>
       </c>
       <c r="R2" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S2" s="14">
         <f>D2+E2</f>
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="U2" s="8"/>
     </row>
@@ -802,46 +814,46 @@
         <v>4</v>
       </c>
       <c r="B3" s="11">
-        <v>45262</v>
+        <v>45332</v>
       </c>
       <c r="C3" s="2">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D3" s="2">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E3" s="2">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="G3" s="2">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H3" s="2">
         <v>0</v>
       </c>
       <c r="I3" s="2">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="J3" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K3" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L3" s="2">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="M3" s="2">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="N3" s="2">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="O3" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3" s="2">
         <v>0</v>
@@ -850,56 +862,56 @@
         <v>0</v>
       </c>
       <c r="R3" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="S3" s="14">
         <f t="shared" ref="S3:S15" si="0">D3+E3</f>
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="U3" s="8"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="11">
-        <v>45265</v>
+        <v>45333</v>
       </c>
       <c r="C4" s="2">
         <v>50</v>
       </c>
       <c r="D4" s="2">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="G4" s="2">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="H4" s="2">
         <v>0</v>
       </c>
       <c r="I4" s="2">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="J4" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K4" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L4" s="2">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="M4" s="2">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="N4" s="2">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="O4" s="2">
         <v>1</v>
@@ -911,59 +923,59 @@
         <v>0</v>
       </c>
       <c r="R4" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="S4" s="14">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="U4" s="8"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="11">
-        <v>45269</v>
+        <v>45347</v>
       </c>
       <c r="C5" s="2">
         <v>15</v>
       </c>
       <c r="D5" s="2">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E5" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="2">
+        <v>10</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>10</v>
+      </c>
+      <c r="J5" s="2">
         <v>3</v>
       </c>
-      <c r="G5" s="2">
-        <v>13</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2">
-        <v>13</v>
-      </c>
-      <c r="J5" s="2">
-        <v>1</v>
-      </c>
       <c r="K5" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5" s="2">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="O5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P5" s="2">
         <v>0</v>
@@ -976,37 +988,37 @@
       </c>
       <c r="S5" s="14">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="U5" s="8"/>
     </row>
     <row r="6" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B6" s="11">
-        <v>45269</v>
+        <v>45332</v>
       </c>
       <c r="C6" s="5">
         <v>90</v>
       </c>
       <c r="D6" s="2">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E6" s="2">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G6" s="5">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="H6" s="5">
         <v>0</v>
       </c>
       <c r="I6" s="5">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J6" s="5">
         <v>0</v>
@@ -1015,74 +1027,74 @@
         <v>0</v>
       </c>
       <c r="L6" s="5">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="M6" s="5">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="N6" s="5">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="O6" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P6" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>0</v>
+      </c>
+      <c r="R6" s="6">
         <v>9</v>
-      </c>
-      <c r="Q6" s="5">
-        <v>0</v>
-      </c>
-      <c r="R6" s="6">
-        <v>24</v>
       </c>
       <c r="S6" s="14">
         <f t="shared" si="0"/>
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="U6" s="9"/>
     </row>
     <row r="7" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="B7" s="11">
-        <v>45277</v>
+        <v>45332</v>
       </c>
       <c r="C7" s="5">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="D7" s="2">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="E7" s="2">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G7" s="5">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="H7" s="5">
         <v>0</v>
       </c>
       <c r="I7" s="5">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="J7" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K7" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L7" s="5">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="M7" s="5">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="N7" s="5">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="O7" s="5">
         <v>0</v>
@@ -1094,26 +1106,26 @@
         <v>0</v>
       </c>
       <c r="R7" s="6">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="S7" s="14">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="U7" s="9"/>
     </row>
     <row r="8" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B8" s="11">
-        <v>45277</v>
+        <v>45339</v>
       </c>
       <c r="C8" s="5">
         <v>30</v>
       </c>
       <c r="D8" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E8" s="2">
         <v>13</v>
@@ -1122,86 +1134,86 @@
         <v>3</v>
       </c>
       <c r="G8" s="5">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H8" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="5">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J8" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K8" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L8" s="5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M8" s="5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="N8" s="5">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="O8" s="5">
         <v>0</v>
       </c>
       <c r="P8" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q8" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R8" s="7">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="S8" s="14">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="U8" s="10"/>
     </row>
     <row r="9" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B9" s="11">
-        <v>45262</v>
+        <v>45326</v>
       </c>
       <c r="C9" s="5">
         <v>80</v>
       </c>
       <c r="D9" s="2">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E9" s="2">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G9" s="5">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="H9" s="5">
         <v>0</v>
       </c>
       <c r="I9" s="5">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="J9" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9" s="5">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="M9" s="5">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="N9" s="5">
         <v>36</v>
@@ -1216,53 +1228,53 @@
         <v>0</v>
       </c>
       <c r="R9" s="6">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="S9" s="14">
         <f t="shared" si="0"/>
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="U9" s="9"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="B10" s="11">
-        <v>45269</v>
+        <v>45347</v>
       </c>
       <c r="C10" s="2">
         <v>15</v>
       </c>
       <c r="D10" s="2">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="E10" s="2">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="G10" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H10" s="2">
         <v>0</v>
       </c>
       <c r="I10" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N10" s="2">
         <v>10</v>
@@ -1277,148 +1289,148 @@
         <v>0</v>
       </c>
       <c r="R10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S10" s="14">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="U10" s="8"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B11" s="11">
-        <v>45263</v>
+        <v>45333</v>
       </c>
       <c r="C11" s="2">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D11" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E11" s="2">
         <v>6</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="G11" s="2">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H11" s="2">
         <v>0</v>
       </c>
       <c r="I11" s="2">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J11" s="2">
+        <v>1</v>
+      </c>
+      <c r="K11" s="2">
+        <v>1</v>
+      </c>
+      <c r="L11" s="2">
+        <v>5</v>
+      </c>
+      <c r="M11" s="2">
+        <v>5</v>
+      </c>
+      <c r="N11" s="2">
+        <v>11</v>
+      </c>
+      <c r="O11" s="2">
+        <v>0</v>
+      </c>
+      <c r="P11" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>0</v>
+      </c>
+      <c r="R11" s="2">
         <v>2</v>
-      </c>
-      <c r="K11" s="2">
-        <v>2</v>
-      </c>
-      <c r="L11" s="2">
-        <v>2</v>
-      </c>
-      <c r="M11" s="2">
-        <v>2</v>
-      </c>
-      <c r="N11" s="2">
-        <v>14</v>
-      </c>
-      <c r="O11" s="2">
-        <v>0</v>
-      </c>
-      <c r="P11" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="2">
-        <v>0</v>
-      </c>
-      <c r="R11" s="2">
-        <v>1</v>
       </c>
       <c r="S11" s="14">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="U11" s="8"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="B12" s="11">
-        <v>45270</v>
+        <v>45340</v>
       </c>
       <c r="C12" s="2">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D12" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="G12" s="2">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H12" s="2">
         <v>0</v>
       </c>
       <c r="I12" s="2">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="J12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12" s="2">
+        <v>1</v>
+      </c>
+      <c r="M12" s="2">
+        <v>1</v>
+      </c>
+      <c r="N12" s="2">
+        <v>11</v>
+      </c>
+      <c r="O12" s="2">
+        <v>0</v>
+      </c>
+      <c r="P12" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>0</v>
+      </c>
+      <c r="R12" s="2">
         <v>2</v>
-      </c>
-      <c r="M12" s="2">
-        <v>2</v>
-      </c>
-      <c r="N12" s="2">
-        <v>20</v>
-      </c>
-      <c r="O12" s="2">
-        <v>0</v>
-      </c>
-      <c r="P12" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="2">
-        <v>0</v>
-      </c>
-      <c r="R12" s="2">
-        <v>3</v>
       </c>
       <c r="S12" s="14">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="U12" s="8"/>
     </row>
     <row r="13" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="B13" s="11">
-        <v>45262</v>
+        <v>45325</v>
       </c>
       <c r="C13" s="5">
         <v>10</v>
       </c>
       <c r="D13" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E13" s="2">
         <v>4</v>
@@ -1427,25 +1439,25 @@
         <v>3</v>
       </c>
       <c r="G13" s="5">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H13" s="5">
         <v>0</v>
       </c>
       <c r="I13" s="5">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J13" s="5">
         <v>0</v>
       </c>
       <c r="K13" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L13" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M13" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13" s="5">
         <v>6</v>
@@ -1454,108 +1466,108 @@
         <v>0</v>
       </c>
       <c r="P13" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q13" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R13" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S13" s="14">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U13" s="9"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="B14" s="11">
-        <v>45270</v>
+        <v>45340</v>
       </c>
       <c r="C14" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D14" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E14" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="2">
+        <v>29</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2">
+        <v>29</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2">
         <v>3</v>
       </c>
-      <c r="G14" s="2">
-        <v>32</v>
-      </c>
-      <c r="H14" s="2">
-        <v>0</v>
-      </c>
-      <c r="I14" s="2">
-        <v>32</v>
-      </c>
-      <c r="J14" s="2">
-        <v>2</v>
-      </c>
-      <c r="K14" s="2">
-        <v>2</v>
-      </c>
-      <c r="L14" s="2">
-        <v>6</v>
-      </c>
       <c r="M14" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="N14" s="2">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="O14" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P14" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q14" s="2">
         <v>0</v>
       </c>
       <c r="R14" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="S14" s="14">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="U14" s="8"/>
     </row>
     <row r="15" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="B15" s="11">
-        <v>45269</v>
+        <v>45332</v>
       </c>
       <c r="C15" s="5">
         <v>30</v>
       </c>
       <c r="D15" s="2">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E15" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G15" s="5">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H15" s="5">
         <v>0</v>
       </c>
       <c r="I15" s="5">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J15" s="5">
         <v>0</v>
@@ -1564,13 +1576,13 @@
         <v>0</v>
       </c>
       <c r="L15" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M15" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N15" s="5">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="O15" s="5">
         <v>0</v>
@@ -1582,11 +1594,11 @@
         <v>0</v>
       </c>
       <c r="R15" s="6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S15" s="14">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="U15" s="9"/>
     </row>

</xml_diff>